<commit_message>
manual matrix placing; additional tests
Ran improved code on 5x10 matrix and 1x2 matrix with finer timestep. Observed reduced error (<0.001%) on 1x2 model with fine timestep and increased error (~0.012%) on 5x10. Mainly when conditions are not stable (at start of simulation). #30
</commit_message>
<xml_diff>
--- a/examples/dev_sandbox/data/mini_grid/placing_matrix_new.xlsx
+++ b/examples/dev_sandbox/data/mini_grid/placing_matrix_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjordan\Documents\GitHub\ClearWater-riverine\examples\dev_sandbox\data\mini_grid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC384E3-3B2A-4BDE-89DD-4419EF612236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFBDD8A-0A75-4327-A41D-5977717810D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48000" yWindow="0" windowWidth="19200" windowHeight="21000" firstSheet="1" activeTab="5" xr2:uid="{0D6685A3-9F3A-4630-99AF-4A1490A22806}"/>
+    <workbookView xWindow="14490" yWindow="-18120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{0D6685A3-9F3A-4630-99AF-4A1490A22806}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Load" sheetId="2" r:id="rId1"/>
@@ -41,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="13">
   <si>
     <t>n+1</t>
   </si>
@@ -87,7 +109,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +129,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -460,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8666B46-C872-40BF-8072-9D3544872922}">
   <dimension ref="B1:M9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M9"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1117,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCAC273-7DB2-44F4-A0A4-6FE5EDD8BB88}">
-  <dimension ref="B1:M9"/>
+  <dimension ref="B1:M18"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1449,6 +1477,63 @@
         <v>6.6666666666666599</v>
       </c>
     </row>
+    <row r="12" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" cm="1">
+        <f t="array" ref="E12:E18">MMULT(MINVERSE(C3:I9), M3:M9)</f>
+        <v>100.00624591923287</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>100.00908943673966</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>100.00026173385577</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>97.018306222898545</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:I1"/>
@@ -1459,15 +1544,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CA6E72-7372-4C3B-AD40-0CE7B3853F9B}">
-  <dimension ref="B1:M9"/>
+  <dimension ref="B1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1489,7 +1574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="3">
         <v>0</v>
       </c>
@@ -1518,36 +1603,36 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3">
         <v>0</v>
       </c>
       <c r="C3">
-        <f>'Total Load'!C3+Advection!C3+Diffusion!C3</f>
+        <f>'Total Load'!C3+Advection!C3+Diffusion!C3+Placeholders!C3</f>
         <v>0.42500830783349564</v>
       </c>
       <c r="D3">
-        <f>'Total Load'!D3+Advection!D3+Diffusion!D3</f>
+        <f>'Total Load'!D3+Advection!D3+Diffusion!D3+Placeholders!D3</f>
         <v>-0.100002250671386</v>
       </c>
       <c r="E3">
-        <f>'Total Load'!E3+Advection!E3+Diffusion!E3</f>
+        <f>'Total Load'!E3+Advection!E3+Diffusion!E3+Placeholders!E3</f>
         <v>0</v>
       </c>
       <c r="F3">
-        <f>'Total Load'!F3+Advection!F3+Diffusion!F3</f>
+        <f>'Total Load'!F3+Advection!F3+Diffusion!F3+Placeholders!F3</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f>'Total Load'!G3+Advection!G3+Diffusion!G3</f>
+        <f>'Total Load'!G3+Advection!G3+Diffusion!G3+Placeholders!G3</f>
         <v>-0.24167120341625001</v>
       </c>
       <c r="H3">
-        <f>'Total Load'!H3+Advection!H3+Diffusion!H3</f>
+        <f>'Total Load'!H3+Advection!H3+Diffusion!H3+Placeholders!H3</f>
         <v>0</v>
       </c>
       <c r="I3">
-        <f>'Total Load'!I3+Advection!I3+Diffusion!I3</f>
+        <f>'Total Load'!I3+Advection!I3+Diffusion!I3+Placeholders!I3</f>
         <v>0</v>
       </c>
       <c r="K3" t="s">
@@ -1557,36 +1642,36 @@
         <v>8.3342552185058505</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4">
-        <f>'Total Load'!C4+Advection!C4+Diffusion!C4</f>
+        <f>'Total Load'!C4+Advection!C4+Diffusion!C4+Placeholders!C4</f>
         <v>-0.141668616671386</v>
       </c>
       <c r="D4">
-        <f>'Total Load'!D4+Advection!D4+Diffusion!D4</f>
+        <f>'Total Load'!D4+Advection!D4+Diffusion!D4+Placeholders!D4</f>
         <v>0.42500382093164057</v>
       </c>
       <c r="E4">
-        <f>'Total Load'!E4+Advection!E4+Diffusion!E4</f>
+        <f>'Total Load'!E4+Advection!E4+Diffusion!E4+Placeholders!E4</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f>'Total Load'!F4+Advection!F4+Diffusion!F4</f>
+        <f>'Total Load'!F4+Advection!F4+Diffusion!F4+Placeholders!F4</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f>'Total Load'!G4+Advection!G4+Diffusion!G4</f>
+        <f>'Total Load'!G4+Advection!G4+Diffusion!G4+Placeholders!G4</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f>'Total Load'!H4+Advection!H4+Diffusion!H4</f>
+        <f>'Total Load'!H4+Advection!H4+Diffusion!H4+Placeholders!H4</f>
         <v>0</v>
       </c>
       <c r="I4">
-        <f>'Total Load'!I4+Advection!I4+Diffusion!I4</f>
+        <f>'Total Load'!I4+Advection!I4+Diffusion!I4+Placeholders!I4</f>
         <v>-0.200001411437988</v>
       </c>
       <c r="K4" t="s">
@@ -1595,37 +1680,49 @@
       <c r="M4">
         <v>8.3342552185058594</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R4">
+        <v>4</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5">
-        <f>'Total Load'!C5+Advection!C5+Diffusion!C5</f>
+        <f>'Total Load'!C5+Advection!C5+Diffusion!C5+Placeholders!C5</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f>'Total Load'!D5+Advection!D5+Diffusion!D5</f>
+        <f>'Total Load'!D5+Advection!D5+Diffusion!D5+Placeholders!D5</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>'Total Load'!E5+Advection!E5+Diffusion!E5</f>
-        <v>0</v>
+        <f>'Total Load'!E5+Advection!E5+Diffusion!E5+Placeholders!E5</f>
+        <v>1</v>
       </c>
       <c r="F5">
-        <f>'Total Load'!F5+Advection!F5+Diffusion!F5</f>
+        <f>'Total Load'!F5+Advection!F5+Diffusion!F5+Placeholders!F5</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f>'Total Load'!G5+Advection!G5+Diffusion!G5</f>
+        <f>'Total Load'!G5+Advection!G5+Diffusion!G5+Placeholders!G5</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f>'Total Load'!H5+Advection!H5+Diffusion!H5</f>
+        <f>'Total Load'!H5+Advection!H5+Diffusion!H5+Placeholders!H5</f>
         <v>0</v>
       </c>
       <c r="I5">
-        <f>'Total Load'!I5+Advection!I5+Diffusion!I5</f>
+        <f>'Total Load'!I5+Advection!I5+Diffusion!I5+Placeholders!I5</f>
         <v>0</v>
       </c>
       <c r="K5" t="s">
@@ -1635,36 +1732,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6">
-        <f>'Total Load'!C6+Advection!C6+Diffusion!C6</f>
+        <f>'Total Load'!C6+Advection!C6+Diffusion!C6+Placeholders!C6</f>
         <v>0</v>
       </c>
       <c r="D6">
-        <f>'Total Load'!D6+Advection!D6+Diffusion!D6</f>
+        <f>'Total Load'!D6+Advection!D6+Diffusion!D6+Placeholders!D6</f>
         <v>0</v>
       </c>
       <c r="E6">
-        <f>'Total Load'!E6+Advection!E6+Diffusion!E6</f>
+        <f>'Total Load'!E6+Advection!E6+Diffusion!E6+Placeholders!E6</f>
         <v>0</v>
       </c>
       <c r="F6">
-        <f>'Total Load'!F6+Advection!F6+Diffusion!F6</f>
-        <v>0</v>
+        <f>'Total Load'!F6+Advection!F6+Diffusion!F6+Placeholders!F6</f>
+        <v>1</v>
       </c>
       <c r="G6">
-        <f>'Total Load'!G6+Advection!G6+Diffusion!G6</f>
+        <f>'Total Load'!G6+Advection!G6+Diffusion!G6+Placeholders!G6</f>
         <v>0</v>
       </c>
       <c r="H6">
-        <f>'Total Load'!H6+Advection!H6+Diffusion!H6</f>
+        <f>'Total Load'!H6+Advection!H6+Diffusion!H6+Placeholders!H6</f>
         <v>0</v>
       </c>
       <c r="I6">
-        <f>'Total Load'!I6+Advection!I6+Diffusion!I6</f>
+        <f>'Total Load'!I6+Advection!I6+Diffusion!I6+Placeholders!I6</f>
         <v>0</v>
       </c>
       <c r="K6" t="s">
@@ -1674,36 +1771,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>4</v>
       </c>
       <c r="C7">
-        <f>'Total Load'!C7+Advection!C7+Diffusion!C7</f>
+        <f>'Total Load'!C7+Advection!C7+Diffusion!C7+Placeholders!C7</f>
         <v>-0.20000452041625899</v>
       </c>
       <c r="D7">
-        <f>'Total Load'!D7+Advection!D7+Diffusion!D7</f>
+        <f>'Total Load'!D7+Advection!D7+Diffusion!D7+Placeholders!D7</f>
         <v>0</v>
       </c>
       <c r="E7">
-        <f>'Total Load'!E7+Advection!E7+Diffusion!E7</f>
+        <f>'Total Load'!E7+Advection!E7+Diffusion!E7+Placeholders!E7</f>
         <v>0</v>
       </c>
       <c r="F7">
-        <f>'Total Load'!F7+Advection!F7+Diffusion!F7</f>
+        <f>'Total Load'!F7+Advection!F7+Diffusion!F7+Placeholders!F7</f>
         <v>0</v>
       </c>
       <c r="G7">
-        <f>'Total Load'!G7+Advection!G7+Diffusion!G7</f>
+        <f>'Total Load'!G7+Advection!G7+Diffusion!G7+Placeholders!G7</f>
         <v>0.31167127971020425</v>
       </c>
       <c r="H7">
-        <f>'Total Load'!H7+Advection!H7+Diffusion!H7</f>
+        <f>'Total Load'!H7+Advection!H7+Diffusion!H7+Placeholders!H7</f>
         <v>0</v>
       </c>
       <c r="I7">
-        <f>'Total Load'!I7+Advection!I7+Diffusion!I7</f>
+        <f>'Total Load'!I7+Advection!I7+Diffusion!I7+Placeholders!I7</f>
         <v>0</v>
       </c>
       <c r="K7" t="s">
@@ -1713,36 +1810,36 @@
         <v>11.166705156366</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>5</v>
       </c>
       <c r="C8">
-        <f>'Total Load'!C8+Advection!C8+Diffusion!C8</f>
+        <f>'Total Load'!C8+Advection!C8+Diffusion!C8+Placeholders!C8</f>
         <v>0</v>
       </c>
       <c r="D8">
-        <f>'Total Load'!D8+Advection!D8+Diffusion!D8</f>
+        <f>'Total Load'!D8+Advection!D8+Diffusion!D8+Placeholders!D8</f>
         <v>0</v>
       </c>
       <c r="E8">
-        <f>'Total Load'!E8+Advection!E8+Diffusion!E8</f>
+        <f>'Total Load'!E8+Advection!E8+Diffusion!E8+Placeholders!E8</f>
         <v>0</v>
       </c>
       <c r="F8">
-        <f>'Total Load'!F8+Advection!F8+Diffusion!F8</f>
+        <f>'Total Load'!F8+Advection!F8+Diffusion!F8+Placeholders!F8</f>
         <v>0</v>
       </c>
       <c r="G8">
-        <f>'Total Load'!G8+Advection!G8+Diffusion!G8</f>
+        <f>'Total Load'!G8+Advection!G8+Diffusion!G8+Placeholders!G8</f>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>'Total Load'!H8+Advection!H8+Diffusion!H8</f>
-        <v>0</v>
+        <f>'Total Load'!H8+Advection!H8+Diffusion!H8+Placeholders!H8</f>
+        <v>1</v>
       </c>
       <c r="I8">
-        <f>'Total Load'!I8+Advection!I8+Diffusion!I8</f>
+        <f>'Total Load'!I8+Advection!I8+Diffusion!I8+Placeholders!I8</f>
         <v>0</v>
       </c>
       <c r="K8" t="s">
@@ -1752,36 +1849,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>6</v>
       </c>
       <c r="C9">
-        <f>'Total Load'!C9+Advection!C9+Diffusion!C9</f>
+        <f>'Total Load'!C9+Advection!C9+Diffusion!C9+Placeholders!C9</f>
         <v>0</v>
       </c>
       <c r="D9">
-        <f>'Total Load'!D8+Advection!D9+Diffusion!D9</f>
+        <f>'Total Load'!D9+Advection!D9+Diffusion!D9+Placeholders!D9</f>
         <v>-0.241667677437988</v>
       </c>
       <c r="E9">
-        <f>'Total Load'!E9+Advection!E9+Diffusion!E9</f>
+        <f>'Total Load'!E9+Advection!E9+Diffusion!E9+Placeholders!E9</f>
         <v>0</v>
       </c>
       <c r="F9">
-        <f>'Total Load'!F9+Advection!F9+Diffusion!F9</f>
+        <f>'Total Load'!F9+Advection!F9+Diffusion!F9+Placeholders!F9</f>
         <v>0</v>
       </c>
       <c r="G9">
-        <f>'Total Load'!G9+Advection!G9+Diffusion!G9</f>
+        <f>'Total Load'!G9+Advection!G9+Diffusion!G9+Placeholders!G9</f>
         <v>0</v>
       </c>
       <c r="H9">
-        <f>'Total Load'!H9+Advection!H9+Diffusion!H9</f>
+        <f>'Total Load'!H9+Advection!H9+Diffusion!H9+Placeholders!H9</f>
         <v>0</v>
       </c>
       <c r="I9">
-        <f>'Total Load'!I9+Advection!I9+Diffusion!I9</f>
+        <f>'Total Load'!I9+Advection!I9+Diffusion!I9+Placeholders!I9</f>
         <v>0.31166767743798801</v>
       </c>
       <c r="K9" t="s">
@@ -1789,13 +1886,72 @@
       </c>
       <c r="M9">
         <v>6.6666666666666599</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" cm="1">
+        <f t="array" ref="E12:E18">MMULT(MINVERSE(C3:I9), M3:M9)</f>
+        <v>99.640672243818003</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>99.022185185899716</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>99.76950731988282</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>98.172285387101937</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:I1"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>